<commit_message>
changes font sizes demographic things
</commit_message>
<xml_diff>
--- a/ILM_WS202223/survey/Immersive-Level-Model Studie (Masterarbeit B. Kurz)(1-28).xlsx
+++ b/ILM_WS202223/survey/Immersive-Level-Model Studie (Masterarbeit B. Kurz)(1-28).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benedikt\Documents\dev\MA_LogParser\logparser\ILM_WS202223\survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC64886-0376-4DD7-A5AB-5699DC184FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B8FC98-32E2-479B-BEE4-466E98E35F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -857,9 +857,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1675,23 +1678,29 @@
   <dimension ref="A1:DR26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F20" sqref="F20"/>
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.77734375" customWidth="1"/>
     <col min="6" max="6" width="50.6640625" customWidth="1"/>
-    <col min="7" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.33203125" customWidth="1"/>
-    <col min="14" max="64" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1"/>
+    <col min="10" max="10" width="76" customWidth="1"/>
+    <col min="11" max="11" width="116.33203125" customWidth="1"/>
+    <col min="12" max="12" width="76" customWidth="1"/>
+    <col min="13" max="13" width="201.88671875" customWidth="1"/>
+    <col min="14" max="14" width="82.77734375" customWidth="1"/>
+    <col min="15" max="64" width="20" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="53.77734375" customWidth="1"/>
     <col min="66" max="122" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:122" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:122" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1725,13 +1734,13 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">

</xml_diff>